<commit_message>
Thêm biểu mẫu, quy định
</commit_message>
<xml_diff>
--- a/docs/YeuCauTuan2/PhanCongTuan2.xlsx
+++ b/docs/YeuCauTuan2/PhanCongTuan2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BaiTap\Project1\docs\YeuCauTuan2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3B403A-7C33-416F-9E36-EC6619709D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68895836-4961-4B44-88A4-266E81AD2D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B9375507-713E-4EEC-9D24-E916973933C5}"/>
   </bookViews>
@@ -69,7 +69,7 @@
     <t>Trương Việt Hoàng</t>
   </si>
   <si>
-    <t>Lập bảng hỏi</t>
+    <t>Còn lại</t>
   </si>
 </sst>
 </file>
@@ -204,7 +204,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">

</xml_diff>